<commit_message>
add UnitTable delete useless item.xlsx add boss and player's combat basic logic
</commit_message>
<xml_diff>
--- a/LubanTools/DesignerConfigs/Datas/__tables__.xlsx
+++ b/LubanTools/DesignerConfigs/Datas/__tables__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GGJ\LubanTools\DesignerConfigs\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\ItisUnreal\LubanTools\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097CFCEB-E202-440E-AFBE-75D6B12B8EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069E3B50-15E5-4F32-83F8-E1891225EEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{947BE16E-96E8-4B86-802B-E77C4FDA60B0}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{947BE16E-96E8-4B86-802B-E77C4FDA60B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,15 +147,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Buffsht</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Buff</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Buffsht@item.xlsx</t>
+    <t>UnitTable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnitTableData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnitTable@unit.xlsx</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -163,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +182,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -210,15 +219,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -228,9 +240,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,20 +562,20 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -597,7 +613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -632,7 +648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -658,7 +674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -668,16 +684,19 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{20BA9020-1355-4D74-A02A-93C9E07C7A47}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>